<commit_message>
manual updates to Wind data
</commit_message>
<xml_diff>
--- a/inst/extdata/generation-consumption-utilization-capacity.xlsx
+++ b/inst/extdata/generation-consumption-utilization-capacity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wind\Desktop\automation\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\CREA-China\monthly snapshot\wind data templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6E1FBF-3C11-4F4E-88FE-ADEA0AB4EAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA23D33F-04C2-4D54-BEF8-E66BA6266D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="1630" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="China_Average Utilization Hours" sheetId="1" r:id="rId1"/>
@@ -287,31 +287,7 @@
     <t>2024-05-30</t>
   </si>
   <si>
-    <t>2000-12:2024-10</t>
-  </si>
-  <si>
-    <t>2018-02:2024-10</t>
-  </si>
-  <si>
-    <t>2008-12:2024-10</t>
-  </si>
-  <si>
-    <t>2018-12:2024-10</t>
-  </si>
-  <si>
-    <t>2020-06:2024-10</t>
-  </si>
-  <si>
-    <t>2017-12:2024-10</t>
-  </si>
-  <si>
-    <t>2021-07:2024-10</t>
-  </si>
-  <si>
     <t>National Energy Administration of the People's Republic of China</t>
-  </si>
-  <si>
-    <t>2024-11-29</t>
   </si>
   <si>
     <t>1989-02:2024-11</t>
@@ -342,6 +318,30 @@
   </si>
   <si>
     <t>2024-12-19</t>
+  </si>
+  <si>
+    <t>2000-12:2024-11</t>
+  </si>
+  <si>
+    <t>2018-02:2024-11</t>
+  </si>
+  <si>
+    <t>2008-12:2024-11</t>
+  </si>
+  <si>
+    <t>2018-12:2024-11</t>
+  </si>
+  <si>
+    <t>2020-06:2024-11</t>
+  </si>
+  <si>
+    <t>2017-12:2024-11</t>
+  </si>
+  <si>
+    <t>2021-07:2024-11</t>
+  </si>
+  <si>
+    <t>2025-01-02</t>
   </si>
 </sst>
 </file>
@@ -770,22 +770,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA439"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J435" sqref="J435"/>
+    <sheetView tabSelected="1" topLeftCell="A434" workbookViewId="0">
+      <selection activeCell="D437" sqref="D437"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="9" max="9" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="str">
         <f>[1]!edb()</f>
         <v>Wind</v>
@@ -905,7 +905,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
     </row>
-    <row r="4" spans="1:27" s="4" customFormat="1" ht="199.5">
+    <row r="4" spans="1:27" s="4" customFormat="1" ht="203">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1242,55 +1242,55 @@
         <v>65</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>66</v>
@@ -1299,25 +1299,25 @@
         <v>67</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="X8" s="5" t="s">
         <v>74</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -1373,7 +1373,7 @@
         <v>69</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>70</v>
@@ -1408,55 +1408,55 @@
         <v>72</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="S10" s="7" t="s">
         <v>73</v>
@@ -1465,25 +1465,25 @@
         <v>73</v>
       </c>
       <c r="U10" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="V10" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="W10" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="X10" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Y10" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="Z10" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="AA10" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -36105,7 +36105,7 @@
         <v>2927</v>
       </c>
       <c r="C428" s="3">
-        <v>4040</v>
+        <v>4041</v>
       </c>
       <c r="D428" s="3">
         <v>1218</v>
@@ -36177,7 +36177,7 @@
         <v>7252</v>
       </c>
       <c r="AA428" s="3">
-        <v>303.39999999999998</v>
+        <v>303.89999999999998</v>
       </c>
     </row>
     <row r="429" spans="1:27">
@@ -37015,25 +37015,25 @@
         <v>45626</v>
       </c>
       <c r="B439" s="3">
-        <v>0</v>
+        <v>3146</v>
       </c>
       <c r="C439" s="3">
-        <v>0</v>
+        <v>3988</v>
       </c>
       <c r="D439" s="3">
-        <v>0</v>
+        <v>1132</v>
       </c>
       <c r="E439" s="3">
-        <v>0</v>
+        <v>6983</v>
       </c>
       <c r="F439" s="3">
-        <v>0</v>
+        <v>1931</v>
       </c>
       <c r="G439" s="3">
-        <v>0</v>
+        <v>4187</v>
       </c>
       <c r="H439" s="3">
-        <v>0</v>
+        <v>2156</v>
       </c>
       <c r="I439" s="3">
         <v>43208</v>
@@ -37048,16 +37048,16 @@
         <v>49218</v>
       </c>
       <c r="M439" s="3">
-        <v>0</v>
+        <v>37516</v>
       </c>
       <c r="N439" s="3">
-        <v>0</v>
+        <v>118669</v>
       </c>
       <c r="O439" s="3">
-        <v>0</v>
+        <v>14270</v>
       </c>
       <c r="P439" s="3">
-        <v>0</v>
+        <v>4580</v>
       </c>
       <c r="Q439" s="3">
         <v>81833</v>

</xml_diff>